<commit_message>
Max News 4 -> 10
기사 기존 4개에서 최대 10개까지 출력 가능
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="현재_통합_문서"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12B414F-CEF9-4965-835D-3F4F5A06660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE77DEDE-2C89-4EAF-94C2-0E423F83E04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2784" yWindow="1512" windowWidth="17904" windowHeight="10248" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="paper" sheetId="11" state="hidden" r:id="rId1"/>
-    <sheet name="internet" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="paper" sheetId="11" r:id="rId1"/>
+    <sheet name="internet" sheetId="4" r:id="rId2"/>
     <sheet name="papPaste" sheetId="10" r:id="rId3"/>
     <sheet name="intPaste" sheetId="9" r:id="rId4"/>
     <sheet name="settings" sheetId="3" state="hidden" r:id="rId5"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>보도시간</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -594,12 +594,138 @@
         <v>신문4링크</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A5)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A5)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A5)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A5)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B5)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B5)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B5)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B5)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B5)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B5)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A6)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A6)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A6)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A6)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B6)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B6)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B6)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B6)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B6)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B6)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A7)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A7)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A7)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A7)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B7)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B7)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B7)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B7)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B7)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B7)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A8)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A8)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A8)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A8)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B8)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B8)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B8)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B8)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B8)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B8)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A9)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A9)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A9)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A9)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B9)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B9)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B9)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B9)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B9)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B9)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A10)*2-2,0)=0,"",OFFSET(papPaste!$A$1,ROW(A10)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(A10)*2-2,1)=0,"",OFFSET(papPaste!$A$1,ROW(A10)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B10)*2-2,2)=0,"",OFFSET(papPaste!$A$1,ROW(B10)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B10)*2-2,3)=0,"",OFFSET(papPaste!$A$1,ROW(B10)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f ca="1">IF(OFFSET(papPaste!$A$1,ROW(B10)*2-1,2)=0,"",OFFSET(papPaste!$A$1,ROW(B10)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -613,7 +739,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E5" sqref="E5:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -713,12 +839,138 @@
         <v>뉴스4링크</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A5)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A5)*2-2,0))</f>
+        <v>2022.09.30.</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A5)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A5)*2-2,1))</f>
+        <v>뉴스4</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B5)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B5)*2-2,2))</f>
+        <v>뉴스4제목</v>
+      </c>
+      <c r="D5" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B5)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B5)*2-2,3))</f>
+        <v>뉴스4내용</v>
+      </c>
+      <c r="E5" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B5)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B5)*2-1,2))</f>
+        <v>뉴스4링크</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A6)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A6)*2-2,0))</f>
+        <v>2022.09.30.</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A6)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A6)*2-2,1))</f>
+        <v>뉴스4</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B6)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B6)*2-2,2))</f>
+        <v>뉴스4제목</v>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B6)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B6)*2-2,3))</f>
+        <v>뉴스4내용</v>
+      </c>
+      <c r="E6" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B6)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B6)*2-1,2))</f>
+        <v>뉴스4링크</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A7)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A7)*2-2,0))</f>
+        <v>2022.09.30.</v>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A7)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A7)*2-2,1))</f>
+        <v>뉴스4</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B7)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B7)*2-2,2))</f>
+        <v>뉴스4제목</v>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B7)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B7)*2-2,3))</f>
+        <v>뉴스4내용</v>
+      </c>
+      <c r="E7" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B7)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B7)*2-1,2))</f>
+        <v>뉴스4링크</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A8)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A8)*2-2,0))</f>
+        <v>2022.09.30.</v>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A8)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A8)*2-2,1))</f>
+        <v>뉴스4</v>
+      </c>
+      <c r="C8" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B8)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B8)*2-2,2))</f>
+        <v>뉴스4제목</v>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B8)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B8)*2-2,3))</f>
+        <v>뉴스4내용</v>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B8)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B8)*2-1,2))</f>
+        <v>뉴스4링크</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A9)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A9)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A9)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A9)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B9)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B9)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B9)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B9)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B9)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B9)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A10)*2-2,0)=0,"",OFFSET(intPaste!$A$1,ROW(A10)*2-2,0))</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(A10)*2-2,1)=0,"",OFFSET(intPaste!$A$1,ROW(A10)*2-2,1))</f>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B10)*2-2,2)=0,"",OFFSET(intPaste!$A$1,ROW(B10)*2-2,2))</f>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B10)*2-2,3)=0,"",OFFSET(intPaste!$A$1,ROW(B10)*2-2,3))</f>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f ca="1">IF(OFFSET(intPaste!$A$1,ROW(B10)*2-1,2)=0,"",OFFSET(intPaste!$A$1,ROW(B10)*2-1,2))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -826,18 +1078,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -846,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C70C31C-FF2C-4CDF-A663-776B3022753F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -942,20 +1194,120 @@
       </c>
       <c r="D8" s="2"/>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>